<commit_message>
Updated style of handle to be circular
</commit_message>
<xml_diff>
--- a/extras/sample_form/slider_label_sample.xlsx
+++ b/extras/sample_form/slider_label_sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\SurveyCTO Plugins\slider-labels\extras\sample_form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BFE1A4-924D-44D9-8251-3341DAE8C9DF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2979BA81-D78B-4032-82A7-9FB9AE6D3578}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -5306,7 +5308,7 @@
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -6252,7 +6254,7 @@
       </c>
       <c r="C2" s="10" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2003131238</v>
+        <v>2003161856</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>

</xml_diff>

<commit_message>
Added ability to store previous value when swipping backwards and forwards
</commit_message>
<xml_diff>
--- a/extras/sample_form/slider_label_sample.xlsx
+++ b/extras/sample_form/slider_label_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\SurveyCTO Plugins\slider-labels\extras\sample_form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2979BA81-D78B-4032-82A7-9FB9AE6D3578}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B3FABA-BE83-4C28-9A7F-968011C08964}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3030,13 +3030,13 @@
     <t>custom-slider-label(min="0", max="10", markers="none")</t>
   </si>
   <si>
-    <t>custom-slider-label(min="0", max="10", markers="labels")</t>
-  </si>
-  <si>
-    <t>custom-slider-label(min="0", max="10", markers="yes")</t>
-  </si>
-  <si>
     <t>.&lt;=7</t>
+  </si>
+  <si>
+    <t>custom-slider-label(min="0", max="20", markers="yes")</t>
+  </si>
+  <si>
+    <t>custom-slider-label(min="0", max="30", markers="labels")</t>
   </si>
 </sst>
 </file>
@@ -3379,7 +3379,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
-  <dxfs count="211">
+  <dxfs count="181">
     <dxf>
       <fill>
         <patternFill>
@@ -4433,13 +4433,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBFB00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
@@ -4450,221 +4443,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAC090"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9CDE5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7E4BD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4BD97"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB3A2C7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9E004F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBFBFBF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6D9E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2DBDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCC1DA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFBFB00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEBF1DE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99BCE7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDCE6F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFCD5B5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFBB57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD44B"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5305,10 +5086,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -5560,7 +5341,7 @@
         <v>389</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>381</v>
@@ -5680,7 +5461,7 @@
         <v>46</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -5690,263 +5471,149 @@
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
-  <conditionalFormatting sqref="I1:I11 F1:F11 F15 I15 B1:C15 B19:C1048576 I19:I1048576 F19:F1048576">
-    <cfRule type="expression" dxfId="210" priority="47">
+  <conditionalFormatting sqref="B1:C15 B19:C1048576 I19:I1048576 F19:F1048576 I1:I15 F1:F15">
+    <cfRule type="expression" dxfId="180" priority="47">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O11 I1:I11 I15 O15 B1:C15 B19:C1048576 O19:O1048576 I19:I1048576">
-    <cfRule type="expression" dxfId="209" priority="48">
+  <conditionalFormatting sqref="B1:C15 B19:C1048576 O19:O1048576 I19:I1048576 O1:O15 I1:I15">
+    <cfRule type="expression" dxfId="179" priority="48">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F11 B1:D11 B15:D15 F15 F19:F1048576 B19:D1048576">
-    <cfRule type="expression" dxfId="208" priority="49">
+  <conditionalFormatting sqref="F19:F1048576 B19:D1048576 F1:F15 B1:D15">
+    <cfRule type="expression" dxfId="178" priority="49">
       <formula>$A1="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:H11 B1:D11 B15:D15 G15:H15 G19:H1048576 B19:D1048576">
-    <cfRule type="expression" dxfId="207" priority="50">
+  <conditionalFormatting sqref="G19:H1048576 B19:D1048576 G1:H15 B1:D15">
+    <cfRule type="expression" dxfId="177" priority="50">
       <formula>$A1="integer"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:H11 B1:D11 B15:D15 G15:H15 G19:H1048576 B19:D1048576">
-    <cfRule type="expression" dxfId="206" priority="51">
+  <conditionalFormatting sqref="G19:H1048576 B19:D1048576 G1:H15 B1:D15">
+    <cfRule type="expression" dxfId="176" priority="51">
       <formula>$A1="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F11 F15 B1:C15 B19:C1048576 F19:F1048576">
-    <cfRule type="expression" dxfId="205" priority="52">
+  <conditionalFormatting sqref="B1:C15 B19:C1048576 F19:F1048576 F1:F15">
+    <cfRule type="expression" dxfId="175" priority="52">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F11 F15 B1:B15 B19:B1048576 F19:F1048576">
-    <cfRule type="expression" dxfId="204" priority="53">
+  <conditionalFormatting sqref="B1:B15 B19:B1048576 F19:F1048576 F1:F15">
+    <cfRule type="expression" dxfId="174" priority="53">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C15 B19:C1048576">
-    <cfRule type="expression" dxfId="203" priority="54">
+    <cfRule type="expression" dxfId="173" priority="54">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="202" priority="55">
+    <cfRule type="expression" dxfId="172" priority="55">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="201" priority="56">
+    <cfRule type="expression" dxfId="171" priority="56">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N11 N15 B1:B15 B19:B1048576 N19:N1048576">
-    <cfRule type="expression" dxfId="200" priority="57">
+  <conditionalFormatting sqref="N1:N11 B1:B15 B19:B1048576 N19:N1048576 N13:N15">
+    <cfRule type="expression" dxfId="170" priority="57">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F11 F15 B1:C15 B19:C1048576 F19:F1048576">
-    <cfRule type="expression" dxfId="199" priority="58">
+  <conditionalFormatting sqref="B1:C15 B19:C1048576 F19:F1048576 F1:F15">
+    <cfRule type="expression" dxfId="169" priority="58">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F11 F15 B1:C15 B19:C1048576 F19:F1048576">
-    <cfRule type="expression" dxfId="198" priority="59">
+  <conditionalFormatting sqref="B1:C15 B19:C1048576 F19:F1048576 F1:F15">
+    <cfRule type="expression" dxfId="168" priority="59">
       <formula>$A1="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C15 B19:C1048576">
-    <cfRule type="expression" dxfId="197" priority="60">
+    <cfRule type="expression" dxfId="167" priority="60">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W11 A15:W15 A19:W1048576">
-    <cfRule type="expression" dxfId="196" priority="61">
+  <conditionalFormatting sqref="A19:W1048576 A1:W15">
+    <cfRule type="expression" dxfId="166" priority="61">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="195" priority="62">
+    <cfRule type="expression" dxfId="165" priority="62">
       <formula>$A1="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="194" priority="63">
+    <cfRule type="expression" dxfId="164" priority="63">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="193" priority="64">
+    <cfRule type="expression" dxfId="163" priority="64">
       <formula>$A1="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="192" priority="65">
+    <cfRule type="expression" dxfId="162" priority="65">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="191" priority="66">
+    <cfRule type="expression" dxfId="161" priority="66">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="190" priority="67">
+    <cfRule type="expression" dxfId="160" priority="67">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="189" priority="68">
+    <cfRule type="expression" dxfId="159" priority="68">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="188" priority="69">
+    <cfRule type="expression" dxfId="158" priority="69">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="187" priority="70">
+    <cfRule type="expression" dxfId="157" priority="70">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="186" priority="71">
+    <cfRule type="expression" dxfId="156" priority="71">
       <formula>OR($A1="username", $A1="phonenumber", $A1="start", $A1="end", $A1="deviceid", $A1="subscriberid", $A1="simserial", $A1="caseid")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="185" priority="72">
+    <cfRule type="expression" dxfId="155" priority="72">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="184" priority="73">
+    <cfRule type="expression" dxfId="154" priority="73">
       <formula>$A1="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="183" priority="74">
+    <cfRule type="expression" dxfId="153" priority="74">
       <formula>$A1="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="182" priority="75">
+    <cfRule type="expression" dxfId="152" priority="75">
       <formula>$A1="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="181" priority="76">
+    <cfRule type="expression" dxfId="151" priority="76">
       <formula>$A1="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="180" priority="77">
+    <cfRule type="expression" dxfId="150" priority="77">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="179" priority="78">
+    <cfRule type="expression" dxfId="149" priority="78">
       <formula>$A1="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="178" priority="79">
+    <cfRule type="expression" dxfId="148" priority="79">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B15 B19:B1048576">
-    <cfRule type="expression" dxfId="177" priority="80">
+    <cfRule type="expression" dxfId="147" priority="80">
       <formula>$A1="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F11 F15 B1:B15 B19:B1048576 F19:F1048576">
-    <cfRule type="expression" dxfId="176" priority="81">
+  <conditionalFormatting sqref="F1:F11 B1:B15 B19:B1048576 F19:F1048576 F13:F15">
+    <cfRule type="expression" dxfId="146" priority="81">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F14 I12:I14 F12:F13">
-    <cfRule type="expression" dxfId="175" priority="82">
-      <formula>$A12="begin group"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14 O12:O14 I12:I13">
-    <cfRule type="expression" dxfId="174" priority="83">
-      <formula>$A12="begin repeat"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14:D14 F12:F14 B12:D13">
-    <cfRule type="expression" dxfId="173" priority="84">
-      <formula>$A12="text"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14:D14 G12:H14 B12:D13">
-    <cfRule type="expression" dxfId="172" priority="85">
-      <formula>$A12="integer"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14:D14 G12:H14 B12:D13">
-    <cfRule type="expression" dxfId="171" priority="86">
-      <formula>$A12="decimal"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12:F14">
-    <cfRule type="expression" dxfId="170" priority="87">
-      <formula>OR(AND(LEFT($A12, 16)="select_multiple ", LEN($A12)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A12, 17)))), AND(LEFT($A12, 11)="select_one ", LEN($A12)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A12, 12)))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12:F14">
-    <cfRule type="expression" dxfId="169" priority="88">
-      <formula>OR($A12="audio audit", $A12="text audit", $A12="speed violations count", $A12="speed violations list", $A12="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N12">
-    <cfRule type="expression" dxfId="168" priority="89">
+    <cfRule type="expression" dxfId="145" priority="89">
       <formula>OR($A12="calculate", $A12="calculate_here")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12:F14">
-    <cfRule type="expression" dxfId="167" priority="90">
-      <formula>OR($A12="date", $A12="datetime")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12:F14">
-    <cfRule type="expression" dxfId="166" priority="91">
-      <formula>$A12="image"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12:W14">
-    <cfRule type="expression" dxfId="165" priority="92">
-      <formula>OR(AND(LEFT($A12, 14)="sensor_stream ", LEN($A12)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A12, 15)))), AND(LEFT($A12, 17)="sensor_statistic ", LEN($A12)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A12, 18)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="164" priority="93">
-      <formula>$A12="comments"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="163" priority="94">
-      <formula>OR($A12="audio", $A12="video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="162" priority="95">
-      <formula>$A12="image"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="161" priority="96">
-      <formula>OR($A12="date", $A12="datetime")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="160" priority="97">
-      <formula>OR($A12="calculate", $A12="calculate_here")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="159" priority="98">
-      <formula>$A12="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="158" priority="99">
-      <formula>$A12="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="157" priority="100">
-      <formula>OR($A12="geopoint", $A12="geoshape", $A12="geotrace")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="156" priority="101">
-      <formula>OR($A12="audio audit", $A12="text audit", $A12="speed violations count", $A12="speed violations list", $A12="speed violations audit")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="155" priority="102">
-      <formula>OR($A12="username", $A12="phonenumber", $A12="start", $A12="end", $A12="deviceid", $A12="subscriberid", $A12="simserial", $A12="caseid")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="154" priority="103">
-      <formula>OR(AND(LEFT($A12, 16)="select_multiple ", LEN($A12)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A12, 17)))), AND(LEFT($A12, 11)="select_one ", LEN($A12)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A12, 12)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="153" priority="104">
-      <formula>$A12="decimal"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="152" priority="105">
-      <formula>$A12="integer"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="151" priority="106">
-      <formula>$A12="text"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="150" priority="107">
-      <formula>$A12="end repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="149" priority="108">
-      <formula>$A12="begin repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="148" priority="109">
-      <formula>$A12="end group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="147" priority="110">
-      <formula>$A12="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="expression" dxfId="146" priority="111">
+    <cfRule type="expression" dxfId="144" priority="111">
       <formula>OR(AND(LEFT($A12, 14)="sensor_stream ", LEN($A12)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A12, 15)))), AND(LEFT($A12, 17)="sensor_statistic ", LEN($A12)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A12, 18)))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F13:F14">
-    <cfRule type="expression" dxfId="145" priority="112">
-      <formula>OR(AND(LEFT($A13, 14)="sensor_stream ", LEN($A13)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A13, 15)))), AND(LEFT($A13, 17)="sensor_statistic ", LEN($A13)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A13, 18)))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N13:N14">
-    <cfRule type="expression" dxfId="144" priority="113">
-      <formula>OR($A13="calculate", $A13="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:C18">
@@ -6254,7 +5921,7 @@
       </c>
       <c r="C2" s="10" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2003161856</v>
+        <v>2003162013</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>

</xml_diff>

<commit_message>
add steps and other parameters.
</commit_message>
<xml_diff>
--- a/extras/sample_form/slider_label_sample.xlsx
+++ b/extras/sample_form/slider_label_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\SurveyCTO Plugins\slider-labels\extras\sample_form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B3FABA-BE83-4C28-9A7F-968011C08964}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9AAA83-49A7-4B14-9998-952C358AF7CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="397">
   <si>
     <t>type</t>
   </si>
@@ -3018,9 +3018,6 @@
     <t>Slide further up</t>
   </si>
   <si>
-    <t>Slider with constraint</t>
-  </si>
-  <si>
     <t>Slider with required value</t>
   </si>
   <si>
@@ -3033,10 +3030,30 @@
     <t>.&lt;=7</t>
   </si>
   <si>
-    <t>custom-slider-label(min="0", max="20", markers="yes")</t>
-  </si>
-  <si>
-    <t>custom-slider-label(min="0", max="30", markers="labels")</t>
+    <t>Slider with constraint 1</t>
+  </si>
+  <si>
+    <t>display_values</t>
+  </si>
+  <si>
+    <t>Value 1 = ${custom_value1}
+Value 2 = ${custom_value2}
+Value 3 = ${custom_value3}
+Value 4 = ${custom_value4}
+Value 5 = ${custom_value5}
+Value 6 = ${custom_value6}</t>
+  </si>
+  <si>
+    <t>custom-slider-label(min="0", max="20", markers="yes", step=2)</t>
+  </si>
+  <si>
+    <t>custom-slider-label(min="0", max="1", markers="none", step=0.1)</t>
+  </si>
+  <si>
+    <t>custom-slider-label(min="0", max="1", markers="labels", step=0.25)</t>
+  </si>
+  <si>
+    <t>custom-slider-label(min="0", max="10", markers="none", step=1, show="yes")</t>
   </si>
 </sst>
 </file>
@@ -5084,12 +5101,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK19"/>
+  <dimension ref="A1:AMK20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14:XFD14"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -5332,16 +5349,16 @@
         <v>44</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>46</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>389</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>390</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>381</v>
@@ -5349,19 +5366,19 @@
     </row>
     <row r="13" spans="1:27">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>115</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>46</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>382</v>
@@ -5378,13 +5395,13 @@
         <v>378</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>46</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>384</v>
@@ -5427,7 +5444,7 @@
         <v>46</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -5444,12 +5461,12 @@
         <v>46</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>43</v>
+        <v>115</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>380</v>
@@ -5461,12 +5478,23 @@
         <v>46</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
         <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="93.6">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -5921,7 +5949,7 @@
       </c>
       <c r="C2" s="10" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2003162013</v>
+        <v>2003191140</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>

</xml_diff>

<commit_message>
remove language from value label
</commit_message>
<xml_diff>
--- a/extras/sample_form/slider_label_sample.xlsx
+++ b/extras/sample_form/slider_label_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\SurveyCTO Plugins\slider-labels\extras\sample_form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9AAA83-49A7-4B14-9998-952C358AF7CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C0F681-7061-428C-9D93-4446B5808E10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3053,7 +3053,7 @@
     <t>custom-slider-label(min="0", max="1", markers="labels", step=0.25)</t>
   </si>
   <si>
-    <t>custom-slider-label(min="0", max="10", markers="none", step=1, show="yes")</t>
+    <t>custom-slider-label(min="0", max="12", markers="none", step=1, show="yes")</t>
   </si>
 </sst>
 </file>
@@ -5949,7 +5949,7 @@
       </c>
       <c r="C2" s="10" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2003191140</v>
+        <v>2003241129</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>

</xml_diff>